<commit_message>
n dimensional euclidean example
</commit_message>
<xml_diff>
--- a/programs/frameworks/neural/data/nb.xlsx
+++ b/programs/frameworks/neural/data/nb.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Documents\Code\objeck-lang\programs\frameworks\neural\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B411479F-63FA-44E4-BB50-EA530ED8F614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF9D76E-E216-49F1-B4F5-4CB02786D7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="696" windowWidth="18060" windowHeight="13920" xr2:uid="{2B653FE1-F82A-4ACE-9CB1-3CA6756D5760}"/>
+    <workbookView xWindow="21012" yWindow="2496" windowWidth="18060" windowHeight="13920" activeTab="1" xr2:uid="{2B653FE1-F82A-4ACE-9CB1-3CA6756D5760}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Naive Bayes" sheetId="1" r:id="rId1"/>
+    <sheet name="K-Nearest Neighbor" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Friend</t>
   </si>
@@ -48,6 +49,33 @@
   </si>
   <si>
     <t>Dear</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>f5</t>
   </si>
 </sst>
 </file>
@@ -401,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A2D949-3F5B-4149-AD76-241343D87915}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +582,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3F9CB3-F997-45DE-8E16-9FAFF1CFE981}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.35</v>
+      </c>
+      <c r="B2">
+        <v>0.91</v>
+      </c>
+      <c r="C2">
+        <v>0.86</v>
+      </c>
+      <c r="D2">
+        <v>0.42</v>
+      </c>
+      <c r="E2">
+        <v>0.71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.21</v>
+      </c>
+      <c r="B3">
+        <v>0.12</v>
+      </c>
+      <c r="C3">
+        <v>0.76</v>
+      </c>
+      <c r="D3">
+        <v>0.22</v>
+      </c>
+      <c r="E3">
+        <v>0.92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.41</v>
+      </c>
+      <c r="B4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C4">
+        <v>0.73</v>
+      </c>
+      <c r="D4">
+        <v>0.21</v>
+      </c>
+      <c r="E4">
+        <v>0.09</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.71</v>
+      </c>
+      <c r="B5">
+        <v>0.34</v>
+      </c>
+      <c r="C5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D5">
+        <v>0.19</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.79</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+      <c r="C6">
+        <v>0.79</v>
+      </c>
+      <c r="D6">
+        <v>0.21</v>
+      </c>
+      <c r="E6">
+        <v>0.44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.61</v>
+      </c>
+      <c r="B7">
+        <v>0.37</v>
+      </c>
+      <c r="C7">
+        <v>0.34</v>
+      </c>
+      <c r="D7">
+        <v>0.81</v>
+      </c>
+      <c r="E7">
+        <v>0.42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.78</v>
+      </c>
+      <c r="B8">
+        <v>0.12</v>
+      </c>
+      <c r="C8">
+        <v>0.31</v>
+      </c>
+      <c r="D8">
+        <v>0.83</v>
+      </c>
+      <c r="E8">
+        <v>0.87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.52</v>
+      </c>
+      <c r="B9">
+        <v>0.23</v>
+      </c>
+      <c r="C9">
+        <v>0.73</v>
+      </c>
+      <c r="D9">
+        <v>0.45</v>
+      </c>
+      <c r="E9">
+        <v>0.78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.53</v>
+      </c>
+      <c r="B10">
+        <v>0.17</v>
+      </c>
+      <c r="C10">
+        <v>0.63</v>
+      </c>
+      <c r="D10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.65</v>
+      </c>
+      <c r="B12">
+        <v>0.78</v>
+      </c>
+      <c r="C12">
+        <v>0.21</v>
+      </c>
+      <c r="D12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>